<commit_message>
140510 modified 6 left
</commit_message>
<xml_diff>
--- a/leetcode.xlsx
+++ b/leetcode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="295">
   <si>
     <t>Two Sum</t>
   </si>
@@ -966,6 +966,50 @@
   </si>
   <si>
     <t>快慢指针，合并排序，递归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从左向右，再从右向左</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f[i]=min{f(1+j)+1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f[i]=f[j] &amp;&amp; s[j+1,i]∈dict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意对*的处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴力过题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f[i][j]=(s[i] eq s[j])&amp;&amp;f[i+1][j-1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>还有O(n)解法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word Break+DFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用哈希表解决</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1042,7 +1086,35 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1331,7 +1403,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1342,7 +1414,7 @@
   <dimension ref="A1:G168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A133" sqref="A1:A1048576"/>
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1381,19 +1453,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>41764</v>
+        <v>41750</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>266</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>267</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
@@ -1401,20 +1473,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>41738</v>
+        <v>41751</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
-        <v>240</v>
+        <v>121</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
@@ -1422,48 +1493,51 @@
         <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>41750</v>
+        <v>41751</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="4">
-        <v>41750</v>
+        <v>41761</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>125</v>
+        <v>246</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
-        <v>41750</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>121</v>
@@ -1472,18 +1546,16 @@
         <v>121</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>217</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B7" s="4">
-        <v>41751</v>
-      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>121</v>
@@ -1492,18 +1564,16 @@
         <v>121</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>227</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B8" s="4">
-        <v>41751</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
-        <v>224</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>121</v>
@@ -1511,19 +1581,15 @@
       <c r="E8" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>142</v>
-      </c>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="B9" s="4">
-        <v>41761</v>
-      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>121</v>
@@ -1531,38 +1597,37 @@
       <c r="E9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>257</v>
-      </c>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="4">
+        <v>41767</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>121</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>121</v>
+        <v>269</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>143</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="4">
+        <v>41767</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>121</v>
@@ -1571,16 +1636,18 @@
         <v>121</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>143</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="4">
+        <v>41767</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>121</v>
@@ -1588,42 +1655,48 @@
       <c r="E12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>1</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="4">
+        <v>41744</v>
+      </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="4">
-        <v>41767</v>
+        <v>41761</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>269</v>
+        <v>121</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
@@ -1631,339 +1704,332 @@
         <v>1</v>
       </c>
       <c r="B15" s="4">
-        <v>41767</v>
+        <v>41737</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>272</v>
-      </c>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>1</v>
       </c>
       <c r="B16" s="4">
-        <v>41767</v>
+        <v>41744</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>121</v>
+        <v>198</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" s="4">
-        <v>41739</v>
+        <v>41744</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>235</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>121</v>
+        <v>198</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>1</v>
       </c>
       <c r="B18" s="4">
+        <v>41746</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4">
         <v>41751</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="4">
-        <v>41753</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>1</v>
       </c>
       <c r="B20" s="4">
-        <v>41762</v>
+        <v>41751</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>1</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="4">
+        <v>41761</v>
+      </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>1</v>
       </c>
-      <c r="B22" s="4">
-        <v>41767</v>
-      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="3" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>121</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>1</v>
       </c>
-      <c r="B23" s="4">
-        <v>41738</v>
-      </c>
+      <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>1</v>
       </c>
-      <c r="B24" s="4">
-        <v>41753</v>
-      </c>
+      <c r="B24" s="2"/>
       <c r="C24" s="3" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>121</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>1</v>
       </c>
       <c r="B25" s="4">
-        <v>41762</v>
+        <v>41768</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>118</v>
+        <v>279</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>1</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="4">
+        <v>41761</v>
+      </c>
       <c r="C26" s="3" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>121</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>1</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>1</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="3" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>1</v>
       </c>
-      <c r="B29" s="4">
-        <v>41764</v>
-      </c>
+      <c r="B29" s="2"/>
       <c r="C29" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>121</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>1</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="4">
+        <v>41762</v>
+      </c>
       <c r="C30" s="3" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>259</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>1</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="3" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>121</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>1</v>
       </c>
       <c r="B32" s="4">
-        <v>41739</v>
+        <v>41755</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>139</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
@@ -1971,19 +2037,19 @@
         <v>1</v>
       </c>
       <c r="B33" s="4">
-        <v>41739</v>
+        <v>41744</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
@@ -1991,19 +2057,19 @@
         <v>1</v>
       </c>
       <c r="B34" s="4">
-        <v>41739</v>
+        <v>41750</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
@@ -2011,19 +2077,19 @@
         <v>1</v>
       </c>
       <c r="B35" s="4">
-        <v>41739</v>
+        <v>41750</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>139</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
@@ -2031,84 +2097,96 @@
         <v>1</v>
       </c>
       <c r="B36" s="4">
-        <v>41758</v>
+        <v>41761</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>136</v>
+        <v>36</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>137</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>1</v>
       </c>
-      <c r="B37" s="2"/>
+      <c r="B37" s="4">
+        <v>41761</v>
+      </c>
       <c r="C37" s="3" t="s">
-        <v>138</v>
+        <v>37</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>139</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>1</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="4">
+        <v>41761</v>
+      </c>
       <c r="C38" s="3" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <v>1</v>
       </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="4">
+        <v>41762</v>
+      </c>
       <c r="C39" s="3" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F39" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>1</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="4">
+        <v>41737</v>
+      </c>
       <c r="C40" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>121</v>
+        <v>176</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -2116,33 +2194,35 @@
       <c r="A41" s="2">
         <v>1</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="4">
+        <v>41737</v>
+      </c>
       <c r="C41" s="3" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>139</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>1</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="4">
+        <v>41738</v>
+      </c>
       <c r="C42" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -2150,57 +2230,47 @@
       <c r="A43" s="2">
         <v>1</v>
       </c>
-      <c r="B43" s="4">
-        <v>41767</v>
-      </c>
+      <c r="B43" s="2"/>
       <c r="C43" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>273</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>1</v>
       </c>
-      <c r="B44" s="4">
-        <v>41746</v>
-      </c>
+      <c r="B44" s="2"/>
       <c r="C44" s="3" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>205</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>1</v>
       </c>
-      <c r="B45" s="4">
-        <v>41750</v>
-      </c>
+      <c r="B45" s="2"/>
       <c r="C45" s="3" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>121</v>
+        <v>182</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>214</v>
+        <v>121</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2209,38 +2279,38 @@
         <v>1</v>
       </c>
       <c r="B46" s="4">
-        <v>41751</v>
+        <v>41755</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>33</v>
+        <v>153</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>121</v>
+        <v>154</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F46" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>1</v>
       </c>
       <c r="B47" s="4">
-        <v>41753</v>
+        <v>41738</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>232</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
@@ -2248,349 +2318,357 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="3" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <v>1</v>
       </c>
       <c r="B49" s="4">
-        <v>41758</v>
+        <v>41768</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <v>1</v>
       </c>
       <c r="B50" s="4">
-        <v>41758</v>
+        <v>41769</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>121</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <v>1</v>
       </c>
       <c r="B51" s="4">
-        <v>41764</v>
+        <v>41739</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>7</v>
+        <v>235</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>263</v>
+        <v>129</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
         <v>1</v>
       </c>
       <c r="B52" s="4">
-        <v>41744</v>
+        <v>41751</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
         <v>1</v>
       </c>
       <c r="B53" s="4">
-        <v>41761</v>
+        <v>41753</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>183</v>
+        <v>121</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
         <v>1</v>
       </c>
       <c r="B54" s="4">
-        <v>41758</v>
+        <v>41762</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>173</v>
+        <v>121</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
         <v>1</v>
       </c>
-      <c r="B55" s="4">
-        <v>41737</v>
-      </c>
+      <c r="B55" s="2"/>
       <c r="C55" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>184</v>
+        <v>121</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A56" s="2">
         <v>1</v>
       </c>
       <c r="B56" s="4">
-        <v>41744</v>
+        <v>41767</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>198</v>
+        <v>121</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
         <v>1</v>
       </c>
       <c r="B57" s="4">
-        <v>41744</v>
+        <v>41738</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>198</v>
+        <v>122</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>123</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
         <v>1</v>
       </c>
       <c r="B58" s="4">
-        <v>41746</v>
+        <v>41750</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>19</v>
+        <v>190</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>184</v>
+        <v>122</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>123</v>
+      </c>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
         <v>1</v>
       </c>
       <c r="B59" s="4">
-        <v>41751</v>
+        <v>41750</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>184</v>
+        <v>122</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
         <v>1</v>
       </c>
       <c r="B60" s="4">
-        <v>41751</v>
+        <v>41768</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>184</v>
+        <v>121</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
         <v>1</v>
       </c>
       <c r="B61" s="4">
-        <v>41761</v>
+        <v>41738</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>184</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
         <v>1</v>
       </c>
-      <c r="B62" s="2"/>
+      <c r="B62" s="4">
+        <v>41738</v>
+      </c>
       <c r="C62" s="3" t="s">
-        <v>86</v>
+        <v>189</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>184</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
         <v>1</v>
       </c>
-      <c r="B63" s="2"/>
+      <c r="B63" s="4">
+        <v>41738</v>
+      </c>
       <c r="C63" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>184</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="G63" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A64" s="2">
         <v>1</v>
       </c>
-      <c r="B64" s="2"/>
+      <c r="B64" s="4">
+        <v>41745</v>
+      </c>
       <c r="C64" s="3" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>184</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A65" s="2">
         <v>1</v>
       </c>
       <c r="B65" s="4">
-        <v>41768</v>
+        <v>41746</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>184</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>279</v>
+        <v>148</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
         <v>1</v>
       </c>
       <c r="B66" s="4">
-        <v>41738</v>
+        <v>41746</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>184</v>
@@ -2598,35 +2676,39 @@
       <c r="E66" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="F66" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A67" s="2">
         <v>1</v>
       </c>
       <c r="B67" s="4">
-        <v>41738</v>
+        <v>41747</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>189</v>
+        <v>98</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>184</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>218</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A68" s="2">
         <v>1</v>
       </c>
       <c r="B68" s="4">
-        <v>41738</v>
+        <v>41751</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>184</v>
@@ -2635,19 +2717,16 @@
         <v>148</v>
       </c>
       <c r="F68" s="2"/>
-      <c r="G68" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+    </row>
+    <row r="69" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A69" s="2">
         <v>1</v>
       </c>
       <c r="B69" s="4">
-        <v>41745</v>
+        <v>41751</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>184</v>
@@ -2655,17 +2734,17 @@
       <c r="E69" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="F69" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A70" s="2">
         <v>1</v>
       </c>
-      <c r="B70" s="4">
-        <v>41746</v>
-      </c>
+      <c r="B70" s="2"/>
       <c r="C70" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>184</v>
@@ -2673,19 +2752,15 @@
       <c r="E70" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A71" s="2">
         <v>1</v>
       </c>
-      <c r="B71" s="4">
-        <v>41746</v>
-      </c>
+      <c r="B71" s="2"/>
       <c r="C71" s="3" t="s">
-        <v>96</v>
+        <v>185</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>184</v>
@@ -2693,39 +2768,31 @@
       <c r="E71" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F71" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A72" s="2">
         <v>1</v>
       </c>
-      <c r="B72" s="4">
-        <v>41747</v>
-      </c>
+      <c r="B72" s="2"/>
       <c r="C72" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>184</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A73" s="2">
         <v>1</v>
       </c>
-      <c r="B73" s="4">
-        <v>41751</v>
-      </c>
+      <c r="B73" s="2"/>
       <c r="C73" s="3" t="s">
-        <v>102</v>
+        <v>186</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>184</v>
@@ -2735,15 +2802,13 @@
       </c>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A74" s="2">
         <v>1</v>
       </c>
-      <c r="B74" s="4">
-        <v>41751</v>
-      </c>
+      <c r="B74" s="2"/>
       <c r="C74" s="3" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>184</v>
@@ -2751,17 +2816,17 @@
       <c r="E74" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F74" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A75" s="2">
         <v>1</v>
       </c>
-      <c r="B75" s="2"/>
+      <c r="B75" s="4">
+        <v>41764</v>
+      </c>
       <c r="C75" s="3" t="s">
-        <v>91</v>
+        <v>250</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>184</v>
@@ -2769,110 +2834,118 @@
       <c r="E75" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F75" s="2"/>
-    </row>
-    <row r="76" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="F75" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A76" s="2">
         <v>1</v>
       </c>
-      <c r="B76" s="2"/>
+      <c r="B76" s="4">
+        <v>41745</v>
+      </c>
       <c r="C76" s="3" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F76" s="2"/>
-    </row>
-    <row r="77" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="F76" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A77" s="2">
         <v>1</v>
       </c>
-      <c r="B77" s="2"/>
+      <c r="B77" s="4">
+        <v>41768</v>
+      </c>
       <c r="C77" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="F77" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A78" s="2">
         <v>1</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="3" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A79" s="2">
         <v>1</v>
       </c>
-      <c r="B79" s="2"/>
+      <c r="B79" s="4">
+        <v>41738</v>
+      </c>
       <c r="C79" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A80" s="2">
         <v>1</v>
       </c>
-      <c r="B80" s="4">
-        <v>41764</v>
-      </c>
+      <c r="B80" s="2"/>
       <c r="C80" s="3" t="s">
-        <v>250</v>
+        <v>155</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F80" s="2" t="s">
-        <v>262</v>
-      </c>
+      <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A81" s="2">
         <v>1</v>
       </c>
       <c r="B81" s="4">
-        <v>41747</v>
+        <v>41762</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>188</v>
+        <v>95</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>219</v>
+        <v>148</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>209</v>
+        <v>255</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
@@ -2880,52 +2953,58 @@
         <v>1</v>
       </c>
       <c r="B82" s="4">
-        <v>41761</v>
+        <v>41738</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>160</v>
+        <v>77</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>245</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A83" s="2">
         <v>1</v>
       </c>
-      <c r="B83" s="2"/>
+      <c r="B83" s="4">
+        <v>41753</v>
+      </c>
       <c r="C83" s="3" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F83" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="84" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A84" s="2">
         <v>1</v>
       </c>
-      <c r="B84" s="2"/>
+      <c r="B84" s="4">
+        <v>41762</v>
+      </c>
       <c r="C84" s="3" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F84" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="85" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A85" s="2">
@@ -2933,13 +3012,13 @@
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="3" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F85" s="2"/>
     </row>
@@ -2947,132 +3026,128 @@
       <c r="A86" s="2">
         <v>1</v>
       </c>
-      <c r="B86" s="4">
-        <v>41745</v>
-      </c>
+      <c r="B86" s="2"/>
       <c r="C86" s="3" t="s">
-        <v>203</v>
+        <v>70</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>204</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A87" s="2">
         <v>1</v>
       </c>
-      <c r="B87" s="4">
-        <v>41768</v>
-      </c>
+      <c r="B87" s="2"/>
       <c r="C87" s="3" t="s">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>278</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A88" s="2">
         <v>1</v>
       </c>
       <c r="B88" s="4">
-        <v>41738</v>
+        <v>41764</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F88" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="89" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A89" s="2">
         <v>1</v>
       </c>
       <c r="B89" s="4">
-        <v>41739</v>
+        <v>41762</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F89" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="90" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A90" s="2">
         <v>1</v>
       </c>
       <c r="B90" s="4">
-        <v>41739</v>
+        <v>41767</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>110</v>
+        <v>169</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F90" s="2"/>
+        <v>277</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="91" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A91" s="2">
         <v>1</v>
       </c>
-      <c r="B91" s="4">
-        <v>41739</v>
-      </c>
+      <c r="B91" s="2"/>
       <c r="C91" s="3" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>194</v>
+        <v>121</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F91" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="92" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A92" s="2">
         <v>1</v>
       </c>
-      <c r="B92" s="4">
-        <v>41750</v>
-      </c>
+      <c r="B92" s="2"/>
       <c r="C92" s="3" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>228</v>
+        <v>120</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>229</v>
+        <v>133</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
@@ -3080,19 +3155,19 @@
         <v>1</v>
       </c>
       <c r="B93" s="4">
-        <v>41751</v>
+        <v>41739</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>214</v>
+        <v>135</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>223</v>
+        <v>139</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
@@ -3100,19 +3175,19 @@
         <v>1</v>
       </c>
       <c r="B94" s="4">
-        <v>41751</v>
+        <v>41739</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>214</v>
+        <v>135</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
@@ -3120,407 +3195,386 @@
         <v>1</v>
       </c>
       <c r="B95" s="4">
-        <v>41752</v>
+        <v>41739</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F95" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="96" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A96" s="2">
         <v>1</v>
       </c>
       <c r="B96" s="4">
-        <v>41753</v>
+        <v>41739</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>231</v>
+        <v>135</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A97" s="2">
         <v>1</v>
       </c>
       <c r="B97" s="4">
-        <v>41764</v>
+        <v>41758</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A98" s="2">
         <v>1</v>
       </c>
-      <c r="B98" s="4">
-        <v>41767</v>
-      </c>
+      <c r="B98" s="2"/>
       <c r="C98" s="3" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A99" s="2">
         <v>1</v>
       </c>
-      <c r="B99" s="4">
-        <v>41762</v>
-      </c>
+      <c r="B99" s="2"/>
       <c r="C99" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A100" s="2">
         <v>1</v>
       </c>
-      <c r="B100" s="4">
-        <v>41739</v>
-      </c>
+      <c r="B100" s="2"/>
       <c r="C100" s="3" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>193</v>
+        <v>121</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A101" s="2">
         <v>1</v>
       </c>
-      <c r="B101" s="4">
-        <v>41751</v>
-      </c>
+      <c r="B101" s="2"/>
       <c r="C101" s="3" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A102" s="2">
         <v>1</v>
       </c>
-      <c r="B102" s="4">
-        <v>41762</v>
-      </c>
+      <c r="B102" s="2"/>
       <c r="C102" s="3" t="s">
-        <v>251</v>
+        <v>16</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>214</v>
+        <v>135</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A103" s="2">
         <v>1</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" s="3" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="D103" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A104" s="2">
+        <v>1</v>
+      </c>
+      <c r="B104" s="4">
+        <v>41767</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A105" s="2">
+        <v>1</v>
+      </c>
+      <c r="B105" s="4">
+        <v>41758</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A106" s="2">
+        <v>1</v>
+      </c>
+      <c r="B106" s="4">
+        <v>41747</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A107" s="2">
+        <v>1</v>
+      </c>
+      <c r="B107" s="4">
+        <v>41758</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A108" s="2">
+        <v>1</v>
+      </c>
+      <c r="B108" s="4">
+        <v>41768</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D108" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F103" s="2"/>
-    </row>
-    <row r="104" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A104" s="2">
-        <v>1</v>
-      </c>
-      <c r="B104" s="4">
-        <v>41755</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A105" s="2">
-        <v>1</v>
-      </c>
-      <c r="B105" s="2"/>
-      <c r="C105" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F105" s="2"/>
-    </row>
-    <row r="106" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A106" s="2">
-        <v>1</v>
-      </c>
-      <c r="B106" s="4">
-        <v>41744</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A107" s="2">
-        <v>1</v>
-      </c>
-      <c r="B107" s="4">
+      <c r="E108" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A109" s="2">
+        <v>1</v>
+      </c>
+      <c r="B109" s="4">
+        <v>41746</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A110" s="2">
+        <v>1</v>
+      </c>
+      <c r="B110" s="4">
         <v>41750</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A108" s="2">
-        <v>1</v>
-      </c>
-      <c r="B108" s="4">
-        <v>41750</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A109" s="2">
-        <v>1</v>
-      </c>
-      <c r="B109" s="4">
-        <v>41761</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A110" s="2">
-        <v>1</v>
-      </c>
-      <c r="B110" s="4">
-        <v>41761</v>
-      </c>
       <c r="C110" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>214</v>
+      </c>
+      <c r="F110" s="2"/>
+    </row>
+    <row r="111" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A111" s="2">
         <v>1</v>
       </c>
       <c r="B111" s="4">
-        <v>41761</v>
+        <v>41751</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
+        <v>214</v>
+      </c>
+      <c r="F111" s="2"/>
+    </row>
+    <row r="112" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A112" s="2">
         <v>1</v>
       </c>
       <c r="B112" s="4">
-        <v>41762</v>
+        <v>41753</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>121</v>
+        <v>231</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A113" s="2">
         <v>1</v>
       </c>
-      <c r="B113" s="4">
-        <v>41755</v>
-      </c>
+      <c r="B113" s="2"/>
       <c r="C113" s="3" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>237</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A114" s="2">
         <v>1</v>
       </c>
       <c r="B114" s="4">
-        <v>41762</v>
+        <v>41738</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>253</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="F114" s="2"/>
     </row>
     <row r="115" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A115" s="2">
         <v>1</v>
       </c>
       <c r="B115" s="4">
-        <v>41737</v>
+        <v>41739</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="F115" s="2"/>
     </row>
@@ -3529,108 +3583,112 @@
         <v>1</v>
       </c>
       <c r="B116" s="4">
-        <v>41750</v>
+        <v>41739</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>215</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A117" s="2">
         <v>1</v>
       </c>
       <c r="B117" s="4">
-        <v>41750</v>
+        <v>41739</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>216</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F117" s="2"/>
     </row>
     <row r="118" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A118" s="2">
         <v>1</v>
       </c>
       <c r="B118" s="4">
-        <v>41737</v>
+        <v>41750</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F118" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="119" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A119" s="2">
         <v>1</v>
       </c>
       <c r="B119" s="4">
-        <v>41738</v>
+        <v>41751</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F119" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="120" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A120" s="2">
         <v>1</v>
       </c>
       <c r="B120" s="4">
-        <v>41753</v>
+        <v>41751</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>178</v>
+        <v>60</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F120" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="121" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A121" s="2">
         <v>1</v>
       </c>
-      <c r="B121" s="2"/>
+      <c r="B121" s="4">
+        <v>41752</v>
+      </c>
       <c r="C121" s="3" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>121</v>
+        <v>231</v>
       </c>
       <c r="F121" s="2"/>
     </row>
@@ -3638,106 +3696,118 @@
       <c r="A122" s="2">
         <v>1</v>
       </c>
-      <c r="B122" s="2"/>
+      <c r="B122" s="4">
+        <v>41753</v>
+      </c>
       <c r="C122" s="3" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F122" s="2"/>
+        <v>231</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="123" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A123" s="2">
         <v>1</v>
       </c>
       <c r="B123" s="4">
-        <v>41758</v>
+        <v>41739</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>242</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F123" s="2"/>
     </row>
     <row r="124" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A124" s="2">
         <v>1</v>
       </c>
-      <c r="B124" s="2"/>
+      <c r="B124" s="4">
+        <v>41751</v>
+      </c>
       <c r="C124" s="3" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F124" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="125" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A125" s="2">
         <v>1</v>
       </c>
       <c r="B125" s="4">
-        <v>41738</v>
+        <v>41762</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>103</v>
+        <v>251</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F125" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="126" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A126" s="2">
         <v>1</v>
       </c>
-      <c r="B126" s="2"/>
+      <c r="B126" s="4">
+        <v>41750</v>
+      </c>
       <c r="C126" s="3" t="s">
-        <v>155</v>
+        <v>30</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F126" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="127" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A127" s="2">
         <v>1</v>
       </c>
       <c r="B127" s="4">
-        <v>41755</v>
+        <v>41750</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>121</v>
+        <v>214</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
@@ -3745,73 +3815,77 @@
         <v>1</v>
       </c>
       <c r="B128" s="4">
-        <v>41755</v>
+        <v>41753</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>45</v>
+        <v>178</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>238</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="F128" s="2"/>
     </row>
     <row r="129" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A129" s="2">
         <v>1</v>
       </c>
       <c r="B129" s="4">
-        <v>41738</v>
+        <v>41755</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F129" s="2"/>
+        <v>239</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="130" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A130" s="2">
         <v>1</v>
       </c>
-      <c r="B130" s="2"/>
+      <c r="B130" s="4">
+        <v>41764</v>
+      </c>
       <c r="C130" s="3" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F130" s="2"/>
+        <v>266</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="131" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A131" s="2">
         <v>1</v>
       </c>
       <c r="B131" s="4">
-        <v>41767</v>
+        <v>41769</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>169</v>
+        <v>9</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>171</v>
+        <v>289</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
@@ -3819,58 +3893,57 @@
         <v>1</v>
       </c>
       <c r="B132" s="4">
-        <v>41752</v>
+        <v>41758</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="F132" s="2"/>
+        <v>243</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="133" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A133" s="2">
         <v>1</v>
       </c>
       <c r="B133" s="4">
-        <v>41762</v>
+        <v>41758</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>255</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="F133" s="2"/>
     </row>
     <row r="134" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A134" s="2">
         <v>1</v>
       </c>
       <c r="B134" s="4">
-        <v>41747</v>
+        <v>41764</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D134" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="E134" s="2" t="s">
-        <v>210</v>
+        <v>263</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G134" s="2" t="s">
-        <v>240</v>
+        <v>261</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
@@ -3878,19 +3951,19 @@
         <v>1</v>
       </c>
       <c r="B135" s="4">
-        <v>41768</v>
+        <v>41764</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>123</v>
+        <v>263</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
@@ -3898,19 +3971,19 @@
         <v>1</v>
       </c>
       <c r="B136" s="4">
-        <v>41768</v>
+        <v>41767</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>157</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>121</v>
+        <v>263</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
@@ -3918,150 +3991,183 @@
         <v>1</v>
       </c>
       <c r="B137" s="4">
-        <v>41768</v>
+        <v>41755</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>162</v>
+        <v>2</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>135</v>
+        <v>230</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>283</v>
+        <v>237</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A138" s="2">
-        <v>0</v>
-      </c>
-      <c r="B138" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B138" s="4">
+        <v>41752</v>
+      </c>
       <c r="C138" s="3" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>117</v>
+        <v>170</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="F138" s="2"/>
     </row>
     <row r="139" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A139" s="2">
-        <v>0</v>
-      </c>
-      <c r="B139" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B139" s="4">
+        <v>41747</v>
+      </c>
       <c r="C139" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>117</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D139" s="2"/>
       <c r="E139" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F139" s="2"/>
+        <v>210</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="140" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A140" s="2">
-        <v>0</v>
-      </c>
-      <c r="B140" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B140" s="4">
+        <v>41769</v>
+      </c>
       <c r="C140" s="3" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F140" s="2"/>
+        <v>263</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="141" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A141" s="2">
-        <v>0</v>
-      </c>
-      <c r="B141" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B141" s="4">
+        <v>41769</v>
+      </c>
       <c r="C141" s="3" t="s">
-        <v>25</v>
+        <v>158</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="F141" s="2"/>
+      <c r="F141" s="2" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="142" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A142" s="2">
-        <v>0</v>
-      </c>
-      <c r="B142" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B142" s="4">
+        <v>41769</v>
+      </c>
       <c r="C142" s="3" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>129</v>
+        <v>263</v>
       </c>
       <c r="F142" s="2"/>
+      <c r="G142" s="2" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="143" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A143" s="2">
-        <v>0</v>
-      </c>
-      <c r="B143" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B143" s="4">
+        <v>41769</v>
+      </c>
       <c r="C143" s="3" t="s">
-        <v>134</v>
+        <v>4</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>135</v>
+        <v>230</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>274</v>
+        <v>291</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A144" s="2">
-        <v>0</v>
-      </c>
-      <c r="B144" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B144" s="4">
+        <v>41769</v>
+      </c>
       <c r="C144" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F144" s="2"/>
+        <v>286</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="145" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A145" s="2">
-        <v>0</v>
-      </c>
-      <c r="B145" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B145" s="4">
+        <v>41769</v>
+      </c>
       <c r="C145" s="3" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>157</v>
+        <v>276</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F145" s="2"/>
+        <v>263</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="146" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A146" s="2">
@@ -4069,13 +4175,13 @@
       </c>
       <c r="B146" s="2"/>
       <c r="C146" s="3" t="s">
-        <v>41</v>
+        <v>116</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F146" s="2"/>
     </row>
@@ -4085,13 +4191,13 @@
       </c>
       <c r="B147" s="2"/>
       <c r="C147" s="3" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>263</v>
+        <v>118</v>
       </c>
       <c r="F147" s="2"/>
     </row>
@@ -4101,13 +4207,13 @@
       </c>
       <c r="B148" s="2"/>
       <c r="C148" s="3" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>276</v>
+        <v>117</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>263</v>
+        <v>120</v>
       </c>
       <c r="F148" s="2"/>
     </row>
@@ -4117,15 +4223,17 @@
       </c>
       <c r="B149" s="2"/>
       <c r="C149" s="3" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="F149" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="150" spans="1:6" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A150" s="2">
@@ -4133,13 +4241,13 @@
       </c>
       <c r="B150" s="2"/>
       <c r="C150" s="3" t="s">
-        <v>159</v>
+        <v>73</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>157</v>
+        <v>288</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
       <c r="F150" s="2"/>
     </row>
@@ -4149,30 +4257,32 @@
       </c>
       <c r="B151" s="2"/>
       <c r="C151" s="3" t="s">
-        <v>4</v>
+        <v>159</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="F151" s="2"/>
+        <v>263</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="153" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="154" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="167" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sortState ref="A2:G168">
-    <sortCondition descending="1" ref="A133"/>
+  <sortState ref="A1:G168">
+    <sortCondition descending="1" ref="A139"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:F151 G46 G117">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A1:F151 G46 G117 G148 G151">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$A1=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$A1=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>